<commit_message>
fix(Event): update column prefixes for consistency
</commit_message>
<xml_diff>
--- a/daten/1 IMPORTS/IMPORT BOT1_Veranstaltungsliste.xlsx
+++ b/daten/1 IMPORTS/IMPORT BOT1_Veranstaltungsliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehsan\Documents\school_project\dot-app\daten\1 IMPORTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9DB874-C440-4C65-8C4D-4F4AE736D97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0483E9-C98B-4886-9866-6E4D0E2C4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">Polizeikommisar*in </t>
   </si>
   <si>
-    <t>Max. Teilnehmer</t>
-  </si>
-  <si>
     <t>Frühester Zeitpunkt</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Min.</t>
+  </si>
+  <si>
+    <t>Max.</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -259,9 +259,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,7 +299,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -405,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -558,10 +558,10 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="1" bestFit="1" customWidth="1"/>
@@ -583,13 +583,13 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
         <v>20</v>
@@ -669,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>20</v>
@@ -729,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -849,10 +849,10 @@
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -860,7 +860,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -869,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1">
         <v>20</v>
@@ -929,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1">
         <v>20</v>
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>